<commit_message>
feat(fastexcel): simplify export util
</commit_message>
<xml_diff>
--- a/i2f-extension/i2f-extension-easyexcel/src/main/resources/assets/excel/map-export-template.xlsx
+++ b/i2f-extension/i2f-extension-easyexcel/src/main/resources/assets/excel/map-export-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,13 +43,28 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -373,13 +389,16 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>